<commit_message>
made chagnes for month append
</commit_message>
<xml_diff>
--- a/ConsolidatedReports.xlsx
+++ b/ConsolidatedReports.xlsx
@@ -402,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -420,6 +420,15 @@
       <c r="D1" t="str">
         <v/>
       </c>
+      <c r="E1" t="str">
+        <v>May-24</v>
+      </c>
+      <c r="F1" t="str">
+        <v/>
+      </c>
+      <c r="G1" t="str">
+        <v/>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -432,6 +441,15 @@
         <v>Rate</v>
       </c>
       <c r="D2" t="str">
+        <v>Value</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Qty</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Rate</v>
+      </c>
+      <c r="G2" t="str">
         <v>Value</v>
       </c>
     </row>
@@ -448,6 +466,15 @@
       <c r="D3" t="str">
         <v/>
       </c>
+      <c r="E3" t="str">
+        <v/>
+      </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
+      <c r="G3" t="str">
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -462,6 +489,15 @@
       <c r="D4">
         <v>16483853</v>
       </c>
+      <c r="E4">
+        <v>173900</v>
+      </c>
+      <c r="F4" t="str">
+        <v>99.44</v>
+      </c>
+      <c r="G4">
+        <v>17292822</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -476,19 +512,37 @@
       <c r="D5">
         <v>10526640</v>
       </c>
+      <c r="E5">
+        <v>141125</v>
+      </c>
+      <c r="F5" t="str">
+        <v>90.99</v>
+      </c>
+      <c r="G5">
+        <v>12840665.54</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
         <v>Sales</v>
       </c>
       <c r="B6">
-        <v>38030</v>
+        <v>37950</v>
       </c>
       <c r="C6" t="str">
-        <v>96.71</v>
+        <v>94.63</v>
       </c>
       <c r="D6">
-        <v>3677881</v>
+        <v>3591209</v>
+      </c>
+      <c r="E6">
+        <v>54225</v>
+      </c>
+      <c r="F6" t="str">
+        <v>90.36</v>
+      </c>
+      <c r="G6">
+        <v>4899771</v>
       </c>
     </row>
     <row r="7">
@@ -504,19 +558,37 @@
       <c r="D7">
         <v>17292822</v>
       </c>
+      <c r="E7">
+        <v>191250</v>
+      </c>
+      <c r="F7" t="str">
+        <v>98.30</v>
+      </c>
+      <c r="G7">
+        <v>18799448</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
         <v>Consumption HDPE</v>
       </c>
       <c r="B8">
-        <v>65595</v>
+        <v>65675</v>
       </c>
       <c r="C8" t="str">
-        <v>92.08</v>
+        <v>93.28</v>
       </c>
       <c r="D8">
-        <v>6039790</v>
+        <v>6126462</v>
+      </c>
+      <c r="E8">
+        <v>69550</v>
+      </c>
+      <c r="F8" t="str">
+        <v>92.51</v>
+      </c>
+      <c r="G8">
+        <v>6434268.539999999</v>
       </c>
     </row>
     <row r="9">
@@ -526,7 +598,7 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>MD</v>
+        <v>MB</v>
       </c>
       <c r="B10" t="str">
         <v/>
@@ -535,6 +607,15 @@
         <v/>
       </c>
       <c r="D10" t="str">
+        <v/>
+      </c>
+      <c r="E10" t="str">
+        <v/>
+      </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+      <c r="G10" t="str">
         <v/>
       </c>
     </row>
@@ -551,6 +632,15 @@
       <c r="D11">
         <v>625575</v>
       </c>
+      <c r="E11">
+        <v>2456</v>
+      </c>
+      <c r="F11" t="str">
+        <v>239.38</v>
+      </c>
+      <c r="G11">
+        <v>587917</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -565,6 +655,15 @@
       <c r="D12">
         <v>154941</v>
       </c>
+      <c r="E12">
+        <v>1254.9</v>
+      </c>
+      <c r="F12" t="str">
+        <v>211.07</v>
+      </c>
+      <c r="G12">
+        <v>264873.1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -579,193 +678,310 @@
       <c r="D13">
         <v>587917</v>
       </c>
+      <c r="E13">
+        <v>2626</v>
+      </c>
+      <c r="F13" t="str">
+        <v>217.47</v>
+      </c>
+      <c r="G13">
+        <v>571082</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v/>
+        <v>Consumption MB</v>
+      </c>
+      <c r="B14">
+        <v>887</v>
+      </c>
+      <c r="C14" t="str">
+        <v>217.14</v>
+      </c>
+      <c r="D14">
+        <v>192599</v>
+      </c>
+      <c r="E14">
+        <v>1084.9</v>
+      </c>
+      <c r="F14" t="str">
+        <v>259.66</v>
+      </c>
+      <c r="G14">
+        <v>281708.1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>CP</v>
-      </c>
-      <c r="B15" t="str">
-        <v/>
-      </c>
-      <c r="C15" t="str">
-        <v/>
-      </c>
-      <c r="D15" t="str">
         <v/>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Opening Stock</v>
-      </c>
-      <c r="B16">
-        <v>46</v>
+        <v>CP</v>
+      </c>
+      <c r="B16" t="str">
+        <v/>
       </c>
       <c r="C16" t="str">
-        <v>2247.35</v>
-      </c>
-      <c r="D16">
-        <v>103378</v>
+        <v/>
+      </c>
+      <c r="D16" t="str">
+        <v/>
+      </c>
+      <c r="E16" t="str">
+        <v/>
+      </c>
+      <c r="F16" t="str">
+        <v/>
+      </c>
+      <c r="G16" t="str">
+        <v/>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Purchase</v>
+        <v>Opening Stock</v>
       </c>
       <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
+        <v>46</v>
+      </c>
+      <c r="C17" t="str">
+        <v>2247.35</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>103378</v>
+      </c>
+      <c r="E17">
+        <v>45</v>
+      </c>
+      <c r="F17" t="str">
+        <v>2243.67</v>
+      </c>
+      <c r="G17">
+        <v>100965</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Closing Stock</v>
+        <v>Purchase</v>
       </c>
       <c r="B18">
-        <v>45</v>
-      </c>
-      <c r="C18" t="str">
-        <v>2243.67</v>
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>100965</v>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v/>
+        <v>Closing Stock</v>
+      </c>
+      <c r="B19">
+        <v>45</v>
+      </c>
+      <c r="C19" t="str">
+        <v>2243.67</v>
+      </c>
+      <c r="D19">
+        <v>100965</v>
+      </c>
+      <c r="E19">
+        <v>45</v>
+      </c>
+      <c r="F19" t="str">
+        <v>2243.69</v>
+      </c>
+      <c r="G19">
+        <v>100966</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>RM Consumption</v>
-      </c>
-      <c r="B20" t="str">
-        <v/>
+        <v>Consumption CP</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
       </c>
       <c r="C20" t="str">
-        <v/>
-      </c>
-      <c r="D20" t="str">
-        <v/>
+        <v>2413.00</v>
+      </c>
+      <c r="D20">
+        <v>2413</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>-1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>Opening Stock</v>
-      </c>
-      <c r="B21">
-        <v>166266</v>
-      </c>
-      <c r="C21" t="str">
-        <v>103.53</v>
-      </c>
-      <c r="D21">
-        <v>17212806</v>
+        <v/>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>Purchase</v>
-      </c>
-      <c r="B22">
-        <v>114648</v>
+        <v>RM Consumption</v>
+      </c>
+      <c r="B22" t="str">
+        <v/>
       </c>
       <c r="C22" t="str">
-        <v>93.17</v>
-      </c>
-      <c r="D22">
-        <v>10681581</v>
+        <v/>
+      </c>
+      <c r="D22" t="str">
+        <v/>
+      </c>
+      <c r="E22" t="str">
+        <v/>
+      </c>
+      <c r="F22" t="str">
+        <v/>
+      </c>
+      <c r="G22" t="str">
+        <v/>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Sales</v>
+        <v>Opening Stock</v>
       </c>
       <c r="B23">
-        <v>38030</v>
+        <v>166266</v>
       </c>
       <c r="C23" t="str">
-        <v>96.71</v>
+        <v>103.53</v>
       </c>
       <c r="D23">
-        <v>3677881</v>
+        <v>17212806</v>
+      </c>
+      <c r="E23">
+        <v>176401</v>
+      </c>
+      <c r="F23" t="str">
+        <v>101.94</v>
+      </c>
+      <c r="G23">
+        <v>17981704</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>Closing Stock</v>
+        <v>Purchase</v>
       </c>
       <c r="B24">
-        <v>176401</v>
+        <v>114648</v>
       </c>
       <c r="C24" t="str">
-        <v>101.94</v>
+        <v>93.17</v>
       </c>
       <c r="D24">
-        <v>17981704</v>
+        <v>10681581</v>
+      </c>
+      <c r="E24">
+        <v>142379.9</v>
+      </c>
+      <c r="F24" t="str">
+        <v>92.05</v>
+      </c>
+      <c r="G24">
+        <v>13105538.639999999</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v/>
+        <v>Sales</v>
+      </c>
+      <c r="B25">
+        <v>37950</v>
+      </c>
+      <c r="C25" t="str">
+        <v>94.63</v>
+      </c>
+      <c r="D25">
+        <v>3591209</v>
+      </c>
+      <c r="E25">
+        <v>54225</v>
+      </c>
+      <c r="F25" t="str">
+        <v>90.36</v>
+      </c>
+      <c r="G25">
+        <v>4899771</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Monofilament</v>
-      </c>
-      <c r="B26" t="str">
-        <v/>
+        <v>Closing Stock</v>
+      </c>
+      <c r="B26">
+        <v>176401</v>
       </c>
       <c r="C26" t="str">
-        <v/>
-      </c>
-      <c r="D26" t="str">
-        <v/>
+        <v>101.94</v>
+      </c>
+      <c r="D26">
+        <v>17981704</v>
+      </c>
+      <c r="E26">
+        <v>193921</v>
+      </c>
+      <c r="F26" t="str">
+        <v>100.41</v>
+      </c>
+      <c r="G26">
+        <v>19471496</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Yarn Purchases</v>
+        <v>Consumption RM</v>
       </c>
       <c r="B27">
-        <v>7124</v>
+        <v>66563</v>
       </c>
       <c r="C27" t="str">
-        <v>120.79</v>
+        <v>94.97</v>
       </c>
       <c r="D27">
-        <v>860500</v>
+        <v>6321474</v>
+      </c>
+      <c r="E27">
+        <v>70634.90000000002</v>
+      </c>
+      <c r="F27" t="str">
+        <v>95.08</v>
+      </c>
+      <c r="G27">
+        <v>6715975.640000001</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>Purchase Fabric</v>
-      </c>
-      <c r="B28">
-        <v>21761</v>
-      </c>
-      <c r="C28" t="str">
-        <v>222.19</v>
-      </c>
-      <c r="D28">
-        <v>4835026.7</v>
+        <v/>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>Consumables Purchase</v>
+        <v>Monofilament</v>
       </c>
       <c r="B29" t="str">
         <v/>
@@ -773,276 +989,474 @@
       <c r="C29" t="str">
         <v/>
       </c>
-      <c r="D29">
-        <v>373440.32</v>
+      <c r="D29" t="str">
+        <v/>
+      </c>
+      <c r="E29" t="str">
+        <v/>
+      </c>
+      <c r="F29" t="str">
+        <v/>
+      </c>
+      <c r="G29" t="str">
+        <v/>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v/>
+        <v>Yarn Purchases</v>
+      </c>
+      <c r="B30">
+        <v>7124</v>
+      </c>
+      <c r="C30" t="str">
+        <v>120.79</v>
+      </c>
+      <c r="D30">
+        <v>860500</v>
+      </c>
+      <c r="E30">
+        <v>11150</v>
+      </c>
+      <c r="F30" t="str">
+        <v>123.65</v>
+      </c>
+      <c r="G30">
+        <v>1378750</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Total COGS</v>
-      </c>
-      <c r="B31" t="str">
-        <v/>
+        <v>Purchase Fabric</v>
+      </c>
+      <c r="B31">
+        <v>21761</v>
       </c>
       <c r="C31" t="str">
-        <v/>
-      </c>
-      <c r="D31" t="str">
-        <v/>
+        <v>222.19</v>
+      </c>
+      <c r="D31">
+        <v>4835026.7</v>
+      </c>
+      <c r="E31">
+        <v>13264.52</v>
+      </c>
+      <c r="F31" t="str">
+        <v>227.57</v>
+      </c>
+      <c r="G31">
+        <v>3018545.8</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>Opening Stock</v>
-      </c>
-      <c r="B32">
-        <v>166266</v>
+        <v>Consumables Purchase</v>
+      </c>
+      <c r="B32" t="str">
+        <v/>
       </c>
       <c r="C32" t="str">
-        <v>103.53</v>
+        <v/>
       </c>
       <c r="D32">
-        <v>17212806</v>
+        <v>373440.32</v>
+      </c>
+      <c r="E32" t="str">
+        <v/>
+      </c>
+      <c r="F32" t="str">
+        <v/>
+      </c>
+      <c r="G32">
+        <v>252347.47</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>Purchase HD</v>
+        <v>Total Purchase</v>
       </c>
       <c r="B33">
-        <v>113950</v>
+        <v>28885</v>
       </c>
       <c r="C33" t="str">
-        <v>92.38</v>
+        <v>210.11</v>
       </c>
       <c r="D33">
-        <v>10526640</v>
+        <v>6068967.0200000005</v>
+      </c>
+      <c r="E33">
+        <v>24414.52</v>
+      </c>
+      <c r="F33" t="str">
+        <v>190.45</v>
+      </c>
+      <c r="G33">
+        <v>4649643.27</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>Purchase MD</v>
+        <v>Consumption Monofil</v>
       </c>
       <c r="B34">
-        <v>698</v>
+        <v>28885</v>
       </c>
       <c r="C34" t="str">
-        <v>221.98</v>
+        <v>210.11</v>
       </c>
       <c r="D34">
-        <v>154941</v>
+        <v>6068967.0200000005</v>
+      </c>
+      <c r="E34">
+        <v>24414.52</v>
+      </c>
+      <c r="F34" t="str">
+        <v>190.45</v>
+      </c>
+      <c r="G34">
+        <v>4649643.27</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>Purchase Monofil</v>
+        <v>Monofil Consumption</v>
       </c>
       <c r="B35">
-        <v>7124</v>
+        <v>95448</v>
       </c>
       <c r="C35" t="str">
-        <v>120.79</v>
+        <v>129.81</v>
       </c>
       <c r="D35">
-        <v>860500</v>
+        <v>12390441.02</v>
+      </c>
+      <c r="E35">
+        <v>95049.42000000003</v>
+      </c>
+      <c r="F35" t="str">
+        <v>119.58</v>
+      </c>
+      <c r="G35">
+        <v>11365618.91</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>RM Sales</v>
-      </c>
-      <c r="B36">
-        <v>38030</v>
-      </c>
-      <c r="C36" t="str">
-        <v>96.71</v>
-      </c>
-      <c r="D36">
-        <v>3677881</v>
+        <v/>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>Closing Stock</v>
-      </c>
-      <c r="B37">
-        <v>176401</v>
+        <v>Total COGS</v>
+      </c>
+      <c r="B37" t="str">
+        <v/>
       </c>
       <c r="C37" t="str">
-        <v>101.94</v>
-      </c>
-      <c r="D37">
-        <v>17981704</v>
+        <v/>
+      </c>
+      <c r="D37" t="str">
+        <v/>
+      </c>
+      <c r="E37" t="str">
+        <v/>
+      </c>
+      <c r="F37" t="str">
+        <v/>
+      </c>
+      <c r="G37" t="str">
+        <v/>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v/>
+        <v>Opening Stock</v>
+      </c>
+      <c r="B38">
+        <v>166266</v>
+      </c>
+      <c r="C38" t="str">
+        <v>103.53</v>
+      </c>
+      <c r="D38">
+        <v>17212806</v>
+      </c>
+      <c r="E38">
+        <v>176401</v>
+      </c>
+      <c r="F38" t="str">
+        <v>101.94</v>
+      </c>
+      <c r="G38">
+        <v>17981704</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>Monofil SFG/FG Opening Stock</v>
-      </c>
-      <c r="B39" t="str">
-        <v/>
+        <v>Purchase HD</v>
+      </c>
+      <c r="B39">
+        <v>113950</v>
       </c>
       <c r="C39" t="str">
-        <v/>
-      </c>
-      <c r="D39" t="str">
-        <v/>
+        <v>92.38</v>
+      </c>
+      <c r="D39">
+        <v>10526640</v>
+      </c>
+      <c r="E39">
+        <v>141125</v>
+      </c>
+      <c r="F39" t="str">
+        <v>90.99</v>
+      </c>
+      <c r="G39">
+        <v>12840665.54</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>SFG Yarn</v>
+        <v>Purchase MD</v>
       </c>
       <c r="B40">
-        <v>98075</v>
+        <v>698</v>
       </c>
       <c r="C40" t="str">
-        <v>165.00</v>
+        <v>221.98</v>
       </c>
       <c r="D40">
-        <v>16182375</v>
+        <v>154941</v>
+      </c>
+      <c r="E40">
+        <v>1254.9</v>
+      </c>
+      <c r="F40" t="str">
+        <v>211.07</v>
+      </c>
+      <c r="G40">
+        <v>264873.1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>FG Fabric</v>
+        <v>Purchase Monofil</v>
       </c>
       <c r="B41">
-        <v>294635</v>
+        <v>7124</v>
       </c>
       <c r="C41" t="str">
-        <v>229.00</v>
+        <v>120.79</v>
       </c>
       <c r="D41">
-        <v>67471415</v>
+        <v>860500</v>
+      </c>
+      <c r="E41">
+        <v>11150</v>
+      </c>
+      <c r="F41" t="str">
+        <v>123.65</v>
+      </c>
+      <c r="G41">
+        <v>1378750</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v/>
+        <v>RM Sales</v>
+      </c>
+      <c r="B42">
+        <v>37950</v>
+      </c>
+      <c r="C42" t="str">
+        <v>94.63</v>
+      </c>
+      <c r="D42">
+        <v>3591209</v>
+      </c>
+      <c r="E42">
+        <v>54225</v>
+      </c>
+      <c r="F42" t="str">
+        <v>90.36</v>
+      </c>
+      <c r="G42">
+        <v>4899771</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>Monofil SFG/FG Purchase</v>
-      </c>
-      <c r="B43" t="str">
-        <v/>
+        <v>Closing Stock</v>
+      </c>
+      <c r="B43">
+        <v>176401</v>
       </c>
       <c r="C43" t="str">
-        <v/>
-      </c>
-      <c r="D43" t="str">
-        <v/>
+        <v>101.94</v>
+      </c>
+      <c r="D43">
+        <v>17981704</v>
+      </c>
+      <c r="E43">
+        <v>193921</v>
+      </c>
+      <c r="F43" t="str">
+        <v>100.41</v>
+      </c>
+      <c r="G43">
+        <v>19471496</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>SFG Yarn</v>
-      </c>
-      <c r="B44">
-        <v>7124</v>
-      </c>
-      <c r="C44" t="str">
-        <v>120.79</v>
-      </c>
-      <c r="D44">
-        <v>860500</v>
+        <v/>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>FG Fabric</v>
-      </c>
-      <c r="B45">
-        <v>21761</v>
+        <v>Monofil SFG/FG Opening Stock</v>
+      </c>
+      <c r="B45" t="str">
+        <v/>
       </c>
       <c r="C45" t="str">
-        <v>222.19</v>
-      </c>
-      <c r="D45">
-        <v>4835026.7</v>
+        <v/>
+      </c>
+      <c r="D45" t="str">
+        <v/>
+      </c>
+      <c r="E45" t="str">
+        <v/>
+      </c>
+      <c r="F45" t="str">
+        <v/>
+      </c>
+      <c r="G45" t="str">
+        <v/>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>Consumables</v>
-      </c>
-      <c r="B46" t="str">
-        <v/>
+        <v>SFG Yarn</v>
+      </c>
+      <c r="B46">
+        <v>98075</v>
       </c>
       <c r="C46" t="str">
-        <v/>
+        <v>165.00</v>
       </c>
       <c r="D46">
-        <v>373440.32</v>
+        <v>16182375</v>
+      </c>
+      <c r="E46">
+        <v>106845</v>
+      </c>
+      <c r="F46" t="str">
+        <v>164.00</v>
+      </c>
+      <c r="G46">
+        <v>17522580</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v/>
+        <v>FG Fabric</v>
+      </c>
+      <c r="B47">
+        <v>294635</v>
+      </c>
+      <c r="C47" t="str">
+        <v>229.00</v>
+      </c>
+      <c r="D47">
+        <v>67471415</v>
+      </c>
+      <c r="E47">
+        <v>286265</v>
+      </c>
+      <c r="F47" t="str">
+        <v>228.00</v>
+      </c>
+      <c r="G47">
+        <v>65268420</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>Monofil SFG/FG Closing Stock</v>
-      </c>
-      <c r="B48" t="str">
-        <v/>
-      </c>
-      <c r="C48" t="str">
-        <v/>
-      </c>
-      <c r="D48" t="str">
         <v/>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>SFG Yarn</v>
-      </c>
-      <c r="B49">
-        <v>106845</v>
+        <v>Monofil SFG/FG Purchase</v>
+      </c>
+      <c r="B49" t="str">
+        <v/>
       </c>
       <c r="C49" t="str">
-        <v>164.00</v>
-      </c>
-      <c r="D49">
-        <v>17522580</v>
+        <v/>
+      </c>
+      <c r="D49" t="str">
+        <v/>
+      </c>
+      <c r="E49" t="str">
+        <v/>
+      </c>
+      <c r="F49" t="str">
+        <v/>
+      </c>
+      <c r="G49" t="str">
+        <v/>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>FG Fabric</v>
+        <v>SFG Yarn</v>
       </c>
       <c r="B50">
-        <v>286265</v>
+        <v>7124</v>
       </c>
       <c r="C50" t="str">
-        <v>228.00</v>
+        <v>120.79</v>
       </c>
       <c r="D50">
-        <v>65268420</v>
+        <v>860500</v>
+      </c>
+      <c r="E50">
+        <v>11150</v>
+      </c>
+      <c r="F50" t="str">
+        <v>123.65</v>
+      </c>
+      <c r="G50">
+        <v>1378750</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v/>
+        <v>FG Fabric</v>
+      </c>
+      <c r="B51">
+        <v>21761</v>
+      </c>
+      <c r="C51" t="str">
+        <v>222.19</v>
+      </c>
+      <c r="D51">
+        <v>4835026.7</v>
+      </c>
+      <c r="E51">
+        <v>13264.52</v>
+      </c>
+      <c r="F51" t="str">
+        <v>227.57</v>
+      </c>
+      <c r="G51">
+        <v>3018545.8</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>Trading COGS</v>
+        <v>Consumables</v>
       </c>
       <c r="B52" t="str">
         <v/>
@@ -1050,62 +1464,200 @@
       <c r="C52" t="str">
         <v/>
       </c>
-      <c r="D52" t="str">
-        <v/>
+      <c r="D52">
+        <v>373440.32</v>
+      </c>
+      <c r="E52" t="str">
+        <v/>
+      </c>
+      <c r="F52" t="str">
+        <v/>
+      </c>
+      <c r="G52">
+        <v>252347.47</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>Opening Stock</v>
-      </c>
-      <c r="B53">
-        <v>848</v>
-      </c>
-      <c r="C53" t="str">
-        <v>218.01</v>
-      </c>
-      <c r="D53">
-        <v>184872</v>
+        <v/>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>Closing Stock</v>
-      </c>
-      <c r="B54">
-        <v>1576</v>
+        <v>Monofil SFG/FG Closing Stock</v>
+      </c>
+      <c r="B54" t="str">
+        <v/>
       </c>
       <c r="C54" t="str">
-        <v>300.33</v>
-      </c>
-      <c r="D54">
-        <v>473318</v>
+        <v/>
+      </c>
+      <c r="D54" t="str">
+        <v/>
+      </c>
+      <c r="E54" t="str">
+        <v/>
+      </c>
+      <c r="F54" t="str">
+        <v/>
+      </c>
+      <c r="G54" t="str">
+        <v/>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
+        <v>SFG Yarn</v>
+      </c>
+      <c r="B55">
+        <v>106845</v>
+      </c>
+      <c r="C55" t="str">
+        <v>164.00</v>
+      </c>
+      <c r="D55">
+        <v>17522580</v>
+      </c>
+      <c r="E55">
+        <v>105229</v>
+      </c>
+      <c r="F55" t="str">
+        <v>163.00</v>
+      </c>
+      <c r="G55">
+        <v>17152327</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>FG Fabric</v>
+      </c>
+      <c r="B56">
+        <v>286265</v>
+      </c>
+      <c r="C56" t="str">
+        <v>228.00</v>
+      </c>
+      <c r="D56">
+        <v>65268420</v>
+      </c>
+      <c r="E56">
+        <v>263759</v>
+      </c>
+      <c r="F56" t="str">
+        <v>219.00</v>
+      </c>
+      <c r="G56">
+        <v>57763289</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>Trading COGS</v>
+      </c>
+      <c r="B58" t="str">
+        <v/>
+      </c>
+      <c r="C58" t="str">
+        <v/>
+      </c>
+      <c r="D58" t="str">
+        <v/>
+      </c>
+      <c r="E58" t="str">
+        <v/>
+      </c>
+      <c r="F58" t="str">
+        <v/>
+      </c>
+      <c r="G58" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>Opening Stock</v>
+      </c>
+      <c r="B59">
+        <v>848</v>
+      </c>
+      <c r="C59" t="str">
+        <v>218.01</v>
+      </c>
+      <c r="D59">
+        <v>184872</v>
+      </c>
+      <c r="E59">
+        <v>1576</v>
+      </c>
+      <c r="F59" t="str">
+        <v>300.33</v>
+      </c>
+      <c r="G59">
+        <v>473318</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>Closing Stock</v>
+      </c>
+      <c r="B60">
+        <v>1576</v>
+      </c>
+      <c r="C60" t="str">
+        <v>300.33</v>
+      </c>
+      <c r="D60">
+        <v>473318</v>
+      </c>
+      <c r="E60">
+        <v>1056</v>
+      </c>
+      <c r="F60" t="str">
+        <v>200.96</v>
+      </c>
+      <c r="G60">
+        <v>212214</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
         <v>Difference Stock</v>
       </c>
-      <c r="B55">
+      <c r="B61">
         <v>728</v>
       </c>
-      <c r="C55" t="str">
+      <c r="C61" t="str">
         <v>396.22</v>
       </c>
-      <c r="D55">
+      <c r="D61">
         <v>288446</v>
+      </c>
+      <c r="E61">
+        <v>520</v>
+      </c>
+      <c r="F61" t="str">
+        <v>502.12</v>
+      </c>
+      <c r="G61">
+        <v>261104</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D55"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G61"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1123,6 +1675,15 @@
       <c r="D1" t="str">
         <v/>
       </c>
+      <c r="E1" t="str">
+        <v>May-24</v>
+      </c>
+      <c r="F1" t="str">
+        <v/>
+      </c>
+      <c r="G1" t="str">
+        <v/>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -1135,6 +1696,15 @@
         <v>Rate</v>
       </c>
       <c r="D2" t="str">
+        <v>Value</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Qty</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Rate</v>
+      </c>
+      <c r="G2" t="str">
         <v>Value</v>
       </c>
     </row>
@@ -1151,6 +1721,15 @@
       <c r="D3">
         <v>101051468</v>
       </c>
+      <c r="E3">
+        <v>571087</v>
+      </c>
+      <c r="F3" t="str">
+        <v>177.29</v>
+      </c>
+      <c r="G3">
+        <v>101246022</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -1165,6 +1744,15 @@
       <c r="D4">
         <v>10681581</v>
       </c>
+      <c r="E4">
+        <v>142379.9</v>
+      </c>
+      <c r="F4" t="str">
+        <v>92.05</v>
+      </c>
+      <c r="G4">
+        <v>13105538.64</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -1179,6 +1767,15 @@
       <c r="D5">
         <v>1164865.8</v>
       </c>
+      <c r="E5">
+        <v>7416.25</v>
+      </c>
+      <c r="F5" t="str">
+        <v>136.27</v>
+      </c>
+      <c r="G5">
+        <v>1010633.4</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -1193,6 +1790,15 @@
       <c r="D6">
         <v>6068967.0200000005</v>
       </c>
+      <c r="E6">
+        <v>24414.52</v>
+      </c>
+      <c r="F6" t="str">
+        <v>190.45</v>
+      </c>
+      <c r="G6">
+        <v>4649643.27</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -1207,6 +1813,15 @@
       <c r="D7">
         <v>101246022</v>
       </c>
+      <c r="E7">
+        <v>563965</v>
+      </c>
+      <c r="F7" t="str">
+        <v>167.74</v>
+      </c>
+      <c r="G7">
+        <v>94599326</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -1221,6 +1836,15 @@
       <c r="D8">
         <v>26939056</v>
       </c>
+      <c r="E8">
+        <v>168227.17</v>
+      </c>
+      <c r="F8" t="str">
+        <v>195.86</v>
+      </c>
+      <c r="G8">
+        <v>32948492</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -1235,6 +1859,15 @@
       <c r="D9">
         <v>34360</v>
       </c>
+      <c r="E9">
+        <v>4134</v>
+      </c>
+      <c r="F9" t="str">
+        <v>10.00</v>
+      </c>
+      <c r="G9">
+        <v>41340</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -1249,6 +1882,15 @@
       <c r="D10">
         <v>2.5</v>
       </c>
+      <c r="E10" t="str">
+        <v/>
+      </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+      <c r="G10">
+        <v>10.94</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -1263,6 +1905,15 @@
       <c r="D11">
         <v>4143559</v>
       </c>
+      <c r="E11" t="str">
+        <v/>
+      </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
+      <c r="G11">
+        <v>4227041</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -1277,6 +1928,15 @@
       <c r="D12">
         <v>685359</v>
       </c>
+      <c r="E12">
+        <v>8271.5</v>
+      </c>
+      <c r="F12" t="str">
+        <v>74.55</v>
+      </c>
+      <c r="G12">
+        <v>616661</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -1291,6 +1951,15 @@
       <c r="D13">
         <v>3594644</v>
       </c>
+      <c r="E13">
+        <v>52769.8</v>
+      </c>
+      <c r="F13" t="str">
+        <v>78.99</v>
+      </c>
+      <c r="G13">
+        <v>4168133</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -1305,6 +1974,15 @@
       <c r="D14">
         <v>125000</v>
       </c>
+      <c r="E14" t="str">
+        <v/>
+      </c>
+      <c r="F14" t="str">
+        <v/>
+      </c>
+      <c r="G14">
+        <v>125000</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -1319,6 +1997,15 @@
       <c r="D15">
         <v>767579</v>
       </c>
+      <c r="E15" t="str">
+        <v/>
+      </c>
+      <c r="F15" t="str">
+        <v/>
+      </c>
+      <c r="G15">
+        <v>1229816</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -1333,6 +2020,15 @@
       <c r="D16">
         <v>8423562</v>
       </c>
+      <c r="E16" t="str">
+        <v/>
+      </c>
+      <c r="F16" t="str">
+        <v/>
+      </c>
+      <c r="G16">
+        <v>9011835</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -1347,6 +2043,15 @@
       <c r="D17">
         <v>9316141</v>
       </c>
+      <c r="E17" t="str">
+        <v/>
+      </c>
+      <c r="F17" t="str">
+        <v/>
+      </c>
+      <c r="G17">
+        <v>10366651</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -1361,17 +2066,26 @@
       <c r="D18">
         <v>63582.31999999285</v>
       </c>
+      <c r="E18" t="str">
+        <v/>
+      </c>
+      <c r="F18" t="str">
+        <v/>
+      </c>
+      <c r="G18">
+        <v>2789319.370000002</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G18"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1389,6 +2103,15 @@
       <c r="D1" t="str">
         <v/>
       </c>
+      <c r="E1" t="str">
+        <v>May-24</v>
+      </c>
+      <c r="F1" t="str">
+        <v/>
+      </c>
+      <c r="G1" t="str">
+        <v/>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -1401,6 +2124,15 @@
         <v>Value</v>
       </c>
       <c r="D2" t="str">
+        <v>Rate</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Qty</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Value</v>
+      </c>
+      <c r="G2" t="str">
         <v>Rate</v>
       </c>
     </row>
@@ -1417,6 +2149,15 @@
       <c r="D3" t="str">
         <v/>
       </c>
+      <c r="E3" t="str">
+        <v/>
+      </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
+      <c r="G3" t="str">
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -1431,6 +2172,15 @@
       <c r="D4" t="str">
         <v/>
       </c>
+      <c r="E4" t="str">
+        <v/>
+      </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
+      <c r="G4" t="str">
+        <v/>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -1445,6 +2195,15 @@
       <c r="D5" t="str">
         <v>252.61</v>
       </c>
+      <c r="E5">
+        <v>43</v>
+      </c>
+      <c r="F5">
+        <v>10400</v>
+      </c>
+      <c r="G5" t="str">
+        <v>241.86</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -1459,6 +2218,15 @@
       <c r="D6" t="str">
         <v/>
       </c>
+      <c r="E6" t="str">
+        <v/>
+      </c>
+      <c r="F6" t="str">
+        <v/>
+      </c>
+      <c r="G6" t="str">
+        <v/>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -1473,6 +2241,15 @@
       <c r="D7" t="str">
         <v>221.51</v>
       </c>
+      <c r="E7">
+        <v>298.25</v>
+      </c>
+      <c r="F7">
+        <v>70710</v>
+      </c>
+      <c r="G7" t="str">
+        <v>237.08</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -1487,6 +2264,15 @@
       <c r="D8" t="str">
         <v>190.00</v>
       </c>
+      <c r="E8">
+        <v>949.42</v>
+      </c>
+      <c r="F8">
+        <v>183407.9</v>
+      </c>
+      <c r="G8" t="str">
+        <v>193.18</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -1501,6 +2287,15 @@
       <c r="D9" t="str">
         <v>140.45</v>
       </c>
+      <c r="E9">
+        <v>6605</v>
+      </c>
+      <c r="F9">
+        <v>978441</v>
+      </c>
+      <c r="G9" t="str">
+        <v>148.14</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -1515,6 +2310,15 @@
       <c r="D10" t="str">
         <v/>
       </c>
+      <c r="E10" t="str">
+        <v/>
+      </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+      <c r="G10" t="str">
+        <v/>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -1529,6 +2333,15 @@
       <c r="D11" t="str">
         <v/>
       </c>
+      <c r="E11" t="str">
+        <v/>
+      </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
+      <c r="G11" t="str">
+        <v/>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -1543,6 +2356,15 @@
       <c r="D12" t="str">
         <v/>
       </c>
+      <c r="E12">
+        <v>549</v>
+      </c>
+      <c r="F12" t="str">
+        <v/>
+      </c>
+      <c r="G12" t="str">
+        <v/>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -1557,6 +2379,15 @@
       <c r="D13" t="str">
         <v>124.56</v>
       </c>
+      <c r="E13">
+        <v>5918</v>
+      </c>
+      <c r="F13">
+        <v>759300</v>
+      </c>
+      <c r="G13" t="str">
+        <v>128.30</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -1571,6 +2402,15 @@
       <c r="D14" t="str">
         <v>195.40</v>
       </c>
+      <c r="E14">
+        <v>298.25</v>
+      </c>
+      <c r="F14">
+        <v>56048</v>
+      </c>
+      <c r="G14" t="str">
+        <v>187.92</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -1585,6 +2425,15 @@
       <c r="D15" t="str">
         <v/>
       </c>
+      <c r="E15" t="str">
+        <v/>
+      </c>
+      <c r="F15" t="str">
+        <v/>
+      </c>
+      <c r="G15" t="str">
+        <v/>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -1599,6 +2448,15 @@
       <c r="D16" t="str">
         <v/>
       </c>
+      <c r="E16" t="str">
+        <v/>
+      </c>
+      <c r="F16" t="str">
+        <v/>
+      </c>
+      <c r="G16" t="str">
+        <v/>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -1613,6 +2471,15 @@
       <c r="D17" t="str">
         <v/>
       </c>
+      <c r="E17" t="str">
+        <v/>
+      </c>
+      <c r="F17" t="str">
+        <v/>
+      </c>
+      <c r="G17" t="str">
+        <v/>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -1627,6 +2494,15 @@
       <c r="D18" t="str">
         <v/>
       </c>
+      <c r="E18" t="str">
+        <v/>
+      </c>
+      <c r="F18" t="str">
+        <v/>
+      </c>
+      <c r="G18" t="str">
+        <v/>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -1641,6 +2517,15 @@
       <c r="D19" t="str">
         <v/>
       </c>
+      <c r="E19" t="str">
+        <v/>
+      </c>
+      <c r="F19" t="str">
+        <v/>
+      </c>
+      <c r="G19" t="str">
+        <v/>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -1655,6 +2540,15 @@
       <c r="D20" t="str">
         <v/>
       </c>
+      <c r="E20" t="str">
+        <v/>
+      </c>
+      <c r="F20" t="str">
+        <v/>
+      </c>
+      <c r="G20" t="str">
+        <v/>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -1669,6 +2563,15 @@
       <c r="D21" t="str">
         <v/>
       </c>
+      <c r="E21" t="str">
+        <v/>
+      </c>
+      <c r="F21" t="str">
+        <v/>
+      </c>
+      <c r="G21" t="str">
+        <v/>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -1683,6 +2586,15 @@
       <c r="D22" t="str">
         <v/>
       </c>
+      <c r="E22" t="str">
+        <v/>
+      </c>
+      <c r="F22" t="str">
+        <v/>
+      </c>
+      <c r="G22" t="str">
+        <v/>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -1697,17 +2609,26 @@
       <c r="D23" t="str">
         <v/>
       </c>
+      <c r="E23" t="str">
+        <v/>
+      </c>
+      <c r="F23" t="str">
+        <v/>
+      </c>
+      <c r="G23" t="str">
+        <v/>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D23"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G23"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1728,6 +2649,18 @@
       <c r="E1" t="str">
         <v/>
       </c>
+      <c r="F1" t="str">
+        <v>May-24</v>
+      </c>
+      <c r="G1" t="str">
+        <v/>
+      </c>
+      <c r="H1" t="str">
+        <v/>
+      </c>
+      <c r="I1" t="str">
+        <v/>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -1743,6 +2676,18 @@
         <v>Value</v>
       </c>
       <c r="E2" t="str">
+        <v>Rate</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Cost %</v>
+      </c>
+      <c r="G2" t="str">
+        <v>Qty</v>
+      </c>
+      <c r="H2" t="str">
+        <v>Value</v>
+      </c>
+      <c r="I2" t="str">
         <v>Rate</v>
       </c>
     </row>
@@ -1762,6 +2707,18 @@
       <c r="E3" t="str">
         <v>103.53</v>
       </c>
+      <c r="F3" t="str">
+        <v>55%</v>
+      </c>
+      <c r="G3">
+        <v>176401</v>
+      </c>
+      <c r="H3">
+        <v>17981704</v>
+      </c>
+      <c r="I3" t="str">
+        <v>101.94</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -1779,6 +2736,18 @@
       <c r="E4" t="str">
         <v>93.17</v>
       </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
+      <c r="G4">
+        <v>142379.9</v>
+      </c>
+      <c r="H4">
+        <v>13105538.64</v>
+      </c>
+      <c r="I4" t="str">
+        <v>92.05</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -1796,6 +2765,18 @@
       <c r="E5" t="str">
         <v>138.82</v>
       </c>
+      <c r="F5" t="str">
+        <v/>
+      </c>
+      <c r="G5">
+        <v>7416</v>
+      </c>
+      <c r="H5">
+        <v>1010633</v>
+      </c>
+      <c r="I5" t="str">
+        <v>136.28</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -1813,6 +2794,18 @@
       <c r="E6" t="str">
         <v>210.11</v>
       </c>
+      <c r="F6" t="str">
+        <v/>
+      </c>
+      <c r="G6">
+        <v>24415</v>
+      </c>
+      <c r="H6">
+        <v>4649643</v>
+      </c>
+      <c r="I6" t="str">
+        <v>190.44</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -1830,6 +2823,18 @@
       <c r="E7" t="str">
         <v>101.94</v>
       </c>
+      <c r="F7" t="str">
+        <v/>
+      </c>
+      <c r="G7">
+        <v>193921</v>
+      </c>
+      <c r="H7">
+        <v>19471496</v>
+      </c>
+      <c r="I7" t="str">
+        <v>100.41</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -1839,13 +2844,25 @@
         <v/>
       </c>
       <c r="C8">
-        <v>38030</v>
+        <v>37950</v>
       </c>
       <c r="D8">
-        <v>3715950</v>
+        <v>3698350</v>
       </c>
       <c r="E8" t="str">
-        <v>97.71</v>
+        <v>97.45</v>
+      </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
+      <c r="G8">
+        <v>54225</v>
+      </c>
+      <c r="H8">
+        <v>5235425</v>
+      </c>
+      <c r="I8" t="str">
+        <v>96.55</v>
       </c>
     </row>
     <row r="9">
@@ -1864,6 +2881,18 @@
       <c r="E9" t="str">
         <v>159.11</v>
       </c>
+      <c r="F9" t="str">
+        <v/>
+      </c>
+      <c r="G9">
+        <v>7896</v>
+      </c>
+      <c r="H9">
+        <v>1242959</v>
+      </c>
+      <c r="I9" t="str">
+        <v>157.42</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -1881,6 +2910,18 @@
       <c r="E10" t="str">
         <v>248.96</v>
       </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+      <c r="G10">
+        <v>24415</v>
+      </c>
+      <c r="H10">
+        <v>6078358</v>
+      </c>
+      <c r="I10" t="str">
+        <v>248.96</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -1890,13 +2931,25 @@
         <v/>
       </c>
       <c r="C11">
-        <v>60486</v>
+        <v>60566</v>
       </c>
       <c r="D11">
-        <v>14812633</v>
+        <v>14830233</v>
       </c>
       <c r="E11" t="str">
-        <v>244.89</v>
+        <v>244.86</v>
+      </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
+      <c r="G11">
+        <v>81691</v>
+      </c>
+      <c r="H11">
+        <v>20391750</v>
+      </c>
+      <c r="I11" t="str">
+        <v>249.62</v>
       </c>
     </row>
     <row r="12">
@@ -1915,6 +2968,18 @@
       <c r="E12" t="str">
         <v/>
       </c>
+      <c r="F12" t="str">
+        <v/>
+      </c>
+      <c r="G12" t="str">
+        <v/>
+      </c>
+      <c r="H12">
+        <v>32948492</v>
+      </c>
+      <c r="I12" t="str">
+        <v/>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -1932,6 +2997,18 @@
       <c r="E13" t="str">
         <v/>
       </c>
+      <c r="F13" t="str">
+        <v/>
+      </c>
+      <c r="G13" t="str">
+        <v/>
+      </c>
+      <c r="H13" t="str">
+        <v/>
+      </c>
+      <c r="I13" t="str">
+        <v/>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -1949,6 +3026,18 @@
       <c r="E14" t="str">
         <v/>
       </c>
+      <c r="F14" t="str">
+        <v/>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="str">
+        <v/>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -1966,6 +3055,18 @@
       <c r="E15" t="str">
         <v>10.00</v>
       </c>
+      <c r="F15" t="str">
+        <v/>
+      </c>
+      <c r="G15">
+        <v>4134</v>
+      </c>
+      <c r="H15">
+        <v>41340</v>
+      </c>
+      <c r="I15" t="str">
+        <v>10.00</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -1983,6 +3084,18 @@
       <c r="E16" t="str">
         <v/>
       </c>
+      <c r="F16" t="str">
+        <v>0%</v>
+      </c>
+      <c r="G16" t="str">
+        <v/>
+      </c>
+      <c r="H16">
+        <v>11</v>
+      </c>
+      <c r="I16" t="str">
+        <v/>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -2000,6 +3113,18 @@
       <c r="E17" t="str">
         <v/>
       </c>
+      <c r="F17" t="str">
+        <v>0%</v>
+      </c>
+      <c r="G17" t="str">
+        <v/>
+      </c>
+      <c r="H17" t="str">
+        <v/>
+      </c>
+      <c r="I17" t="str">
+        <v/>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -2017,6 +3142,18 @@
       <c r="E18" t="str">
         <v/>
       </c>
+      <c r="F18" t="str">
+        <v>0%</v>
+      </c>
+      <c r="G18" t="str">
+        <v/>
+      </c>
+      <c r="H18" t="str">
+        <v/>
+      </c>
+      <c r="I18" t="str">
+        <v/>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -2034,6 +3171,18 @@
       <c r="E19" t="str">
         <v>102.84</v>
       </c>
+      <c r="F19" t="str">
+        <v>2%</v>
+      </c>
+      <c r="G19">
+        <v>8271.5</v>
+      </c>
+      <c r="H19">
+        <v>616661</v>
+      </c>
+      <c r="I19" t="str">
+        <v>74.55</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -2051,6 +3200,18 @@
       <c r="E20" t="str">
         <v>78.86</v>
       </c>
+      <c r="F20" t="str">
+        <v>13%</v>
+      </c>
+      <c r="G20">
+        <v>52769.8</v>
+      </c>
+      <c r="H20">
+        <v>4168133</v>
+      </c>
+      <c r="I20" t="str">
+        <v>78.99</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -2068,6 +3229,18 @@
       <c r="E21" t="str">
         <v/>
       </c>
+      <c r="F21" t="str">
+        <v>15%</v>
+      </c>
+      <c r="G21" t="str">
+        <v/>
+      </c>
+      <c r="H21" t="str">
+        <v/>
+      </c>
+      <c r="I21" t="str">
+        <v/>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -2085,6 +3258,18 @@
       <c r="E22" t="str">
         <v/>
       </c>
+      <c r="F22" t="str">
+        <v>0%</v>
+      </c>
+      <c r="G22" t="str">
+        <v/>
+      </c>
+      <c r="H22" t="str">
+        <v/>
+      </c>
+      <c r="I22" t="str">
+        <v/>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -2102,6 +3287,18 @@
       <c r="E23" t="str">
         <v/>
       </c>
+      <c r="F23" t="str">
+        <v>0%</v>
+      </c>
+      <c r="G23" t="str">
+        <v/>
+      </c>
+      <c r="H23" t="str">
+        <v/>
+      </c>
+      <c r="I23" t="str">
+        <v/>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -2119,6 +3316,18 @@
       <c r="E24" t="str">
         <v/>
       </c>
+      <c r="F24" t="str">
+        <v>0%</v>
+      </c>
+      <c r="G24" t="str">
+        <v/>
+      </c>
+      <c r="H24" t="str">
+        <v/>
+      </c>
+      <c r="I24" t="str">
+        <v/>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -2136,6 +3345,18 @@
       <c r="E25" t="str">
         <v/>
       </c>
+      <c r="F25" t="str">
+        <v>0%</v>
+      </c>
+      <c r="G25" t="str">
+        <v/>
+      </c>
+      <c r="H25" t="str">
+        <v/>
+      </c>
+      <c r="I25" t="str">
+        <v/>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -2153,6 +3374,18 @@
       <c r="E26" t="str">
         <v/>
       </c>
+      <c r="F26" t="str">
+        <v/>
+      </c>
+      <c r="G26" t="str">
+        <v/>
+      </c>
+      <c r="H26" t="str">
+        <v/>
+      </c>
+      <c r="I26" t="str">
+        <v/>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -2170,6 +3403,18 @@
       <c r="E27" t="str">
         <v/>
       </c>
+      <c r="F27" t="str">
+        <v>0%</v>
+      </c>
+      <c r="G27" t="str">
+        <v/>
+      </c>
+      <c r="H27">
+        <v>125000</v>
+      </c>
+      <c r="I27" t="str">
+        <v/>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -2187,6 +3432,18 @@
       <c r="E28" t="str">
         <v/>
       </c>
+      <c r="F28" t="str">
+        <v>0%</v>
+      </c>
+      <c r="G28" t="str">
+        <v/>
+      </c>
+      <c r="H28" t="str">
+        <v/>
+      </c>
+      <c r="I28" t="str">
+        <v/>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -2204,6 +3461,18 @@
       <c r="E29" t="str">
         <v/>
       </c>
+      <c r="F29" t="str">
+        <v>0%</v>
+      </c>
+      <c r="G29" t="str">
+        <v/>
+      </c>
+      <c r="H29" t="str">
+        <v/>
+      </c>
+      <c r="I29" t="str">
+        <v/>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -2221,6 +3490,18 @@
       <c r="E30" t="str">
         <v/>
       </c>
+      <c r="F30" t="str">
+        <v>0%</v>
+      </c>
+      <c r="G30" t="str">
+        <v/>
+      </c>
+      <c r="H30" t="str">
+        <v/>
+      </c>
+      <c r="I30" t="str">
+        <v/>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -2238,6 +3519,18 @@
       <c r="E31" t="str">
         <v/>
       </c>
+      <c r="F31" t="str">
+        <v>0%</v>
+      </c>
+      <c r="G31" t="str">
+        <v/>
+      </c>
+      <c r="H31" t="str">
+        <v/>
+      </c>
+      <c r="I31" t="str">
+        <v/>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -2255,6 +3548,18 @@
       <c r="E32" t="str">
         <v/>
       </c>
+      <c r="F32" t="str">
+        <v>0%</v>
+      </c>
+      <c r="G32" t="str">
+        <v/>
+      </c>
+      <c r="H32" t="str">
+        <v/>
+      </c>
+      <c r="I32" t="str">
+        <v/>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -2272,6 +3577,18 @@
       <c r="E33" t="str">
         <v/>
       </c>
+      <c r="F33" t="str">
+        <v>0%</v>
+      </c>
+      <c r="G33" t="str">
+        <v/>
+      </c>
+      <c r="H33" t="str">
+        <v/>
+      </c>
+      <c r="I33" t="str">
+        <v/>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -2289,6 +3606,18 @@
       <c r="E34" t="str">
         <v/>
       </c>
+      <c r="F34" t="str">
+        <v>15%</v>
+      </c>
+      <c r="G34" t="str">
+        <v/>
+      </c>
+      <c r="H34" t="str">
+        <v/>
+      </c>
+      <c r="I34" t="str">
+        <v/>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
@@ -2306,17 +3635,29 @@
       <c r="E35" t="str">
         <v/>
       </c>
+      <c r="F35" t="str">
+        <v/>
+      </c>
+      <c r="G35" t="str">
+        <v/>
+      </c>
+      <c r="H35" t="str">
+        <v/>
+      </c>
+      <c r="I35" t="str">
+        <v/>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E35"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I35"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2418,13 +3759,13 @@
         <v>Apr-24</v>
       </c>
       <c r="B2">
-        <v>22003843</v>
+        <v>22021443</v>
       </c>
       <c r="C2">
         <v>1219263</v>
       </c>
       <c r="D2">
-        <v>3715950</v>
+        <v>3698350</v>
       </c>
       <c r="E2">
         <v>26939056</v>
@@ -2433,10 +3774,10 @@
         <v>34363</v>
       </c>
       <c r="G2">
-        <v>6234802</v>
+        <v>6321474</v>
       </c>
       <c r="H2" t="str">
-        <v>36%</v>
+        <v>37%</v>
       </c>
       <c r="I2">
         <v>6068967.0200000005</v>
@@ -2445,7 +3786,7 @@
         <v>862790</v>
       </c>
       <c r="K2">
-        <v>13166559.02</v>
+        <v>13253231.02</v>
       </c>
       <c r="L2" t="str">
         <v>77%</v>
@@ -2457,7 +3798,7 @@
         <v>288446</v>
       </c>
       <c r="O2">
-        <v>3677881</v>
+        <v>3591209</v>
       </c>
       <c r="P2">
         <v>17132886.02</v>
@@ -2505,16 +3846,108 @@
         <v>4468836.98</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>May-24</v>
+      </c>
+      <c r="B3">
+        <v>26470108</v>
+      </c>
+      <c r="C3">
+        <v>1242959</v>
+      </c>
+      <c r="D3">
+        <v>5235425</v>
+      </c>
+      <c r="E3">
+        <v>32948492</v>
+      </c>
+      <c r="F3">
+        <v>41351</v>
+      </c>
+      <c r="G3">
+        <v>6715975.640000001</v>
+      </c>
+      <c r="H3" t="str">
+        <v>28%</v>
+      </c>
+      <c r="I3">
+        <v>4649643.27</v>
+      </c>
+      <c r="J3">
+        <v>7875384</v>
+      </c>
+      <c r="K3">
+        <v>19241002.91</v>
+      </c>
+      <c r="L3" t="str">
+        <v>79%</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>261104</v>
+      </c>
+      <c r="O3">
+        <v>4899771</v>
+      </c>
+      <c r="P3">
+        <v>24401877.91</v>
+      </c>
+      <c r="Q3" t="str">
+        <v>100%</v>
+      </c>
+      <c r="R3">
+        <v>744437</v>
+      </c>
+      <c r="S3" t="str">
+        <v>3%</v>
+      </c>
+      <c r="T3">
+        <v>564180</v>
+      </c>
+      <c r="U3" t="str">
+        <v>2%</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>1308617</v>
+      </c>
+      <c r="X3" t="str">
+        <v>5%</v>
+      </c>
+      <c r="Y3">
+        <v>7279348.09</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="str">
+        <v>0%</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="str">
+        <v>0%</v>
+      </c>
+      <c r="AD3">
+        <v>7279348.09</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AD2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AD3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AT3"/>
+  <dimension ref="A1:AT4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2885,13 +4318,13 @@
         <v>160.46</v>
       </c>
       <c r="AF3">
-        <v>38030</v>
+        <v>37950</v>
       </c>
       <c r="AG3">
-        <v>3715950</v>
+        <v>3698350</v>
       </c>
       <c r="AH3" t="str">
-        <v>97.71</v>
+        <v>97.45</v>
       </c>
       <c r="AI3">
         <v>3436</v>
@@ -2921,18 +4354,158 @@
         <v/>
       </c>
       <c r="AR3">
-        <v>41466</v>
+        <v>41386</v>
       </c>
       <c r="AS3">
-        <v>3750310</v>
+        <v>3732710</v>
       </c>
       <c r="AT3" t="str">
-        <v>90.44</v>
+        <v>90.19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>May-24</v>
+      </c>
+      <c r="B4">
+        <v>53859.21</v>
+      </c>
+      <c r="C4">
+        <v>14054692</v>
+      </c>
+      <c r="D4" t="str">
+        <v>260.95</v>
+      </c>
+      <c r="E4">
+        <v>41654.76</v>
+      </c>
+      <c r="F4">
+        <v>10900743.2</v>
+      </c>
+      <c r="G4" t="str">
+        <v>261.69</v>
+      </c>
+      <c r="H4">
+        <v>10.02</v>
+      </c>
+      <c r="I4">
+        <v>6750</v>
+      </c>
+      <c r="J4" t="str">
+        <v>673.65</v>
+      </c>
+      <c r="K4">
+        <v>9050</v>
+      </c>
+      <c r="L4">
+        <v>1190125</v>
+      </c>
+      <c r="M4" t="str">
+        <v>131.51</v>
+      </c>
+      <c r="N4">
+        <v>104573.99</v>
+      </c>
+      <c r="O4">
+        <v>26152310.2</v>
+      </c>
+      <c r="P4" t="str">
+        <v>250.08</v>
+      </c>
+      <c r="Q4">
+        <v>298.25</v>
+      </c>
+      <c r="R4">
+        <v>70710</v>
+      </c>
+      <c r="S4" t="str">
+        <v>237.08</v>
+      </c>
+      <c r="T4">
+        <v>42.9</v>
+      </c>
+      <c r="U4">
+        <v>10400</v>
+      </c>
+      <c r="V4" t="str">
+        <v>242.42</v>
+      </c>
+      <c r="W4">
+        <v>2141.45</v>
+      </c>
+      <c r="X4">
+        <v>489460.69999999995</v>
+      </c>
+      <c r="Y4" t="str">
+        <v>228.57</v>
+      </c>
+      <c r="Z4">
+        <v>6605</v>
+      </c>
+      <c r="AA4">
+        <v>978441</v>
+      </c>
+      <c r="AB4" t="str">
+        <v>148.14</v>
+      </c>
+      <c r="AC4">
+        <v>9087.6</v>
+      </c>
+      <c r="AD4">
+        <v>1549011.7</v>
+      </c>
+      <c r="AE4" t="str">
+        <v>170.45</v>
+      </c>
+      <c r="AF4">
+        <v>54225</v>
+      </c>
+      <c r="AG4">
+        <v>5235425</v>
+      </c>
+      <c r="AH4" t="str">
+        <v>96.55</v>
+      </c>
+      <c r="AI4">
+        <v>4134</v>
+      </c>
+      <c r="AJ4">
+        <v>41340</v>
+      </c>
+      <c r="AK4" t="str">
+        <v>10.00</v>
+      </c>
+      <c r="AL4" t="str">
+        <v/>
+      </c>
+      <c r="AM4" t="str">
+        <v/>
+      </c>
+      <c r="AN4" t="str">
+        <v/>
+      </c>
+      <c r="AO4" t="str">
+        <v/>
+      </c>
+      <c r="AP4" t="str">
+        <v/>
+      </c>
+      <c r="AQ4" t="str">
+        <v/>
+      </c>
+      <c r="AR4">
+        <v>58359</v>
+      </c>
+      <c r="AS4">
+        <v>5276765</v>
+      </c>
+      <c r="AT4" t="str">
+        <v>90.42</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AT3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AT4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>